<commit_message>
LED Sequencer Schematic and PCB
</commit_message>
<xml_diff>
--- a/Component.xlsx
+++ b/Component.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alice\Desktop\Altium_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB6B518-DD0F-4BFE-B9C2-612CBE66436A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D97083C-8D2E-4536-A9DA-886DD3636227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3920" yWindow="670" windowWidth="15250" windowHeight="10490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -138,13 +138,13 @@
     <t>Murata</t>
   </si>
   <si>
-    <t>capacitors</t>
-  </si>
-  <si>
     <t>Harwin</t>
   </si>
   <si>
     <t>M20-9990246</t>
+  </si>
+  <si>
+    <t>capacitors 1uF</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -716,7 +716,7 @@
         <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1" t="s">
@@ -732,15 +732,15 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="F14" s="1">
         <v>1</v>

</xml_diff>